<commit_message>
Updating the dummy data with negative content
</commit_message>
<xml_diff>
--- a/data/dummy/Parliament_Members.xlsx
+++ b/data/dummy/Parliament_Members.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentmatton/climact_dev/hackaton_ecf_aim/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\hackaton_20241106\hackaton_ecf_aim\data\dummy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{550FCEDA-4AF9-9B4B-96F4-378717E4C91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F80575-DDE5-4264-9A17-59067484BD03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parliament_Members" sheetId="1" r:id="rId1"/>
     <sheet name="Content" sheetId="2" r:id="rId2"/>
+    <sheet name="Votes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="88">
   <si>
     <t>ID</t>
   </si>
@@ -280,6 +281,24 @@
   </si>
   <si>
     <t>City</t>
+  </si>
+  <si>
+    <t>New measures are not needed to support industries affected by the transition.</t>
+  </si>
+  <si>
+    <t>I believe this policy is not necessary to combat climate change.</t>
+  </si>
+  <si>
+    <t>The current measures are enough to support industries affected by the transition.</t>
+  </si>
+  <si>
+    <t>Public opinion is stable so nothing needs to change.</t>
+  </si>
+  <si>
+    <t>Climate change is a hoax.</t>
+  </si>
+  <si>
+    <t>I don't believe this policy is necessary to combat climate change.</t>
   </si>
 </sst>
 </file>
@@ -341,12 +360,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,23 +674,23 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection sqref="A1:C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -699,7 +719,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -725,7 +745,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -751,7 +771,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -777,7 +797,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -803,7 +823,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -829,7 +849,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -855,7 +875,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -881,7 +901,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -907,7 +927,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -933,7 +953,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -959,7 +979,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -985,7 +1005,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1011,7 +1031,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1037,7 +1057,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1063,7 +1083,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1089,7 +1109,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1115,7 +1135,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1141,7 +1161,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1167,7 +1187,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1193,7 +1213,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1226,24 +1246,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A723DD-D67E-4948-A2E2-642C128126FD}">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="68.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1266,7 +1287,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1289,7 +1310,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1312,7 +1333,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1335,7 +1356,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1357,8 +1378,9 @@
       <c r="G5" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1380,8 +1402,9 @@
       <c r="G6" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1401,10 +1424,10 @@
         <v>75</v>
       </c>
       <c r="G7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1424,10 +1447,10 @@
         <v>75</v>
       </c>
       <c r="G8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1447,10 +1470,10 @@
         <v>75</v>
       </c>
       <c r="G9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1470,10 +1493,10 @@
         <v>75</v>
       </c>
       <c r="G10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1493,10 +1516,10 @@
         <v>75</v>
       </c>
       <c r="G11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1519,7 +1542,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1539,10 +1562,10 @@
         <v>75</v>
       </c>
       <c r="G13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1565,7 +1588,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>3</v>
       </c>
@@ -1588,7 +1611,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3</v>
       </c>
@@ -1611,7 +1634,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1634,7 +1657,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4</v>
       </c>
@@ -1657,7 +1680,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4</v>
       </c>
@@ -1680,7 +1703,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>4</v>
       </c>
@@ -1703,7 +1726,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>4</v>
       </c>
@@ -1726,7 +1749,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>5</v>
       </c>
@@ -1749,7 +1772,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>5</v>
       </c>
@@ -1772,7 +1795,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>5</v>
       </c>
@@ -1795,7 +1818,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>5</v>
       </c>
@@ -1818,7 +1841,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>5</v>
       </c>
@@ -1841,7 +1864,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>6</v>
       </c>
@@ -1864,7 +1887,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>6</v>
       </c>
@@ -1887,7 +1910,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>6</v>
       </c>
@@ -1910,7 +1933,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>6</v>
       </c>
@@ -1933,7 +1956,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>6</v>
       </c>
@@ -1956,7 +1979,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>7</v>
       </c>
@@ -1979,7 +2002,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>7</v>
       </c>
@@ -2002,7 +2025,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>7</v>
       </c>
@@ -2025,7 +2048,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>7</v>
       </c>
@@ -2048,7 +2071,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>7</v>
       </c>
@@ -2071,7 +2094,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>8</v>
       </c>
@@ -2094,7 +2117,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>8</v>
       </c>
@@ -2117,7 +2140,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>8</v>
       </c>
@@ -2140,7 +2163,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>8</v>
       </c>
@@ -2163,7 +2186,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>8</v>
       </c>
@@ -2186,7 +2209,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>9</v>
       </c>
@@ -2209,7 +2232,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>9</v>
       </c>
@@ -2232,7 +2255,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>9</v>
       </c>
@@ -2255,7 +2278,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>9</v>
       </c>
@@ -2278,7 +2301,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>9</v>
       </c>
@@ -2301,7 +2324,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>10</v>
       </c>
@@ -2324,7 +2347,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>10</v>
       </c>
@@ -2347,7 +2370,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>10</v>
       </c>
@@ -2370,7 +2393,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>10</v>
       </c>
@@ -2393,7 +2416,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>10</v>
       </c>
@@ -2416,7 +2439,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>11</v>
       </c>
@@ -2439,7 +2462,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>11</v>
       </c>
@@ -2462,7 +2485,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>11</v>
       </c>
@@ -2485,7 +2508,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>11</v>
       </c>
@@ -2508,7 +2531,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>11</v>
       </c>
@@ -2531,7 +2554,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>12</v>
       </c>
@@ -2554,7 +2577,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>12</v>
       </c>
@@ -2577,7 +2600,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>12</v>
       </c>
@@ -2600,7 +2623,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>12</v>
       </c>
@@ -2623,7 +2646,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>12</v>
       </c>
@@ -2646,7 +2669,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>13</v>
       </c>
@@ -2669,7 +2692,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>13</v>
       </c>
@@ -2692,7 +2715,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>13</v>
       </c>
@@ -2715,7 +2738,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>13</v>
       </c>
@@ -2738,7 +2761,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>13</v>
       </c>
@@ -2761,7 +2784,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>14</v>
       </c>
@@ -2784,7 +2807,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>14</v>
       </c>
@@ -2807,7 +2830,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>14</v>
       </c>
@@ -2830,7 +2853,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>14</v>
       </c>
@@ -2853,7 +2876,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>14</v>
       </c>
@@ -2876,7 +2899,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>15</v>
       </c>
@@ -2899,7 +2922,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>15</v>
       </c>
@@ -2922,7 +2945,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>15</v>
       </c>
@@ -2945,7 +2968,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>15</v>
       </c>
@@ -2968,7 +2991,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>15</v>
       </c>
@@ -2991,7 +3014,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>16</v>
       </c>
@@ -3014,7 +3037,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>16</v>
       </c>
@@ -3037,7 +3060,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>16</v>
       </c>
@@ -3060,7 +3083,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>16</v>
       </c>
@@ -3083,7 +3106,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>16</v>
       </c>
@@ -3106,7 +3129,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>17</v>
       </c>
@@ -3129,7 +3152,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>17</v>
       </c>
@@ -3152,7 +3175,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>17</v>
       </c>
@@ -3175,7 +3198,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>17</v>
       </c>
@@ -3198,7 +3221,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>17</v>
       </c>
@@ -3221,7 +3244,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>18</v>
       </c>
@@ -3244,7 +3267,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>18</v>
       </c>
@@ -3267,7 +3290,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>18</v>
       </c>
@@ -3290,7 +3313,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>18</v>
       </c>
@@ -3313,7 +3336,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>18</v>
       </c>
@@ -3336,7 +3359,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>19</v>
       </c>
@@ -3359,7 +3382,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>19</v>
       </c>
@@ -3382,7 +3405,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>19</v>
       </c>
@@ -3405,7 +3428,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>19</v>
       </c>
@@ -3428,7 +3451,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>19</v>
       </c>
@@ -3451,7 +3474,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>20</v>
       </c>
@@ -3474,7 +3497,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>20</v>
       </c>
@@ -3497,7 +3520,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>20</v>
       </c>
@@ -3520,7 +3543,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>20</v>
       </c>
@@ -3543,7 +3566,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>20</v>
       </c>
@@ -3564,6 +3587,393 @@
       </c>
       <c r="G101" t="s">
         <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C94F8BB3-C833-4D34-B02A-55149437192D}">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>45323</v>
+      </c>
+      <c r="E1" s="3">
+        <v>45439</v>
+      </c>
+      <c r="F1" s="3">
+        <v>45610</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding score to the sentiment analysis
</commit_message>
<xml_diff>
--- a/data/dummy/Parliament_Members.xlsx
+++ b/data/dummy/Parliament_Members.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/D/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\hackaton_20241106\hackaton_ecf_aim\data\dummy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC1A360-984B-B84B-BDDE-546EA8EAA344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8034049F-25E0-455D-89DF-AAD2CB1BDBD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="23260" windowHeight="12460" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parliament_Members" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="116">
   <si>
     <t>ID</t>
   </si>
@@ -138,9 +138,6 @@
   </si>
   <si>
     <t>Germany</t>
-  </si>
-  <si>
-    <t>UK</t>
   </si>
   <si>
     <t>Chamber of Deputies</t>
@@ -488,7 +485,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -792,24 +789,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -823,7 +820,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -838,7 +835,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -852,19 +849,19 @@
         <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H2">
         <v>46</v>
       </c>
       <c r="I2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -878,19 +875,19 @@
         <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H3">
         <v>38</v>
       </c>
       <c r="I3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -904,19 +901,19 @@
         <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H4">
         <v>53</v>
       </c>
       <c r="I4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -930,19 +927,19 @@
         <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H5">
         <v>66</v>
       </c>
       <c r="I5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -953,22 +950,22 @@
         <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H6">
         <v>33</v>
       </c>
       <c r="I6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -982,19 +979,19 @@
         <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H7">
         <v>49</v>
       </c>
       <c r="I7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1008,19 +1005,19 @@
         <v>31</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H8">
         <v>49</v>
       </c>
       <c r="I8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1031,22 +1028,22 @@
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H9">
         <v>67</v>
       </c>
       <c r="I9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1060,19 +1057,19 @@
         <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H10">
         <v>54</v>
       </c>
       <c r="I10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1083,19 +1080,19 @@
         <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H11">
         <v>63</v>
       </c>
       <c r="I11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1111,19 +1108,19 @@
       <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="68.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1146,7 +1143,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1160,16 +1157,16 @@
         <v>45455</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" t="s">
         <v>55</v>
       </c>
-      <c r="G2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1183,16 +1180,16 @@
         <v>45307</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" t="s">
         <v>55</v>
       </c>
-      <c r="G3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1206,16 +1203,16 @@
         <v>45392</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1229,17 +1226,17 @@
         <v>45490</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1253,17 +1250,17 @@
         <v>45480</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1277,16 +1274,16 @@
         <v>45409</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1300,16 +1297,16 @@
         <v>45477</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1323,16 +1320,16 @@
         <v>45431</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1346,16 +1343,16 @@
         <v>45518</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1369,16 +1366,16 @@
         <v>45376</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1392,16 +1389,16 @@
         <v>45585</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" t="s">
         <v>55</v>
       </c>
-      <c r="G12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1415,16 +1412,16 @@
         <v>45328</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1438,16 +1435,16 @@
         <v>45532</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>3</v>
       </c>
@@ -1461,16 +1458,16 @@
         <v>45389</v>
       </c>
       <c r="E15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3</v>
       </c>
@@ -1484,16 +1481,16 @@
         <v>45498</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1507,16 +1504,16 @@
         <v>45349</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4</v>
       </c>
@@ -1530,16 +1527,16 @@
         <v>45412</v>
       </c>
       <c r="E18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4</v>
       </c>
@@ -1553,16 +1550,16 @@
         <v>45575</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>4</v>
       </c>
@@ -1576,16 +1573,16 @@
         <v>45320</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G20" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>5</v>
       </c>
@@ -1599,16 +1596,16 @@
         <v>45475</v>
       </c>
       <c r="E21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G21" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>5</v>
       </c>
@@ -1622,16 +1619,16 @@
         <v>45509</v>
       </c>
       <c r="E22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G22" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>5</v>
       </c>
@@ -1645,16 +1642,16 @@
         <v>45331</v>
       </c>
       <c r="E23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>5</v>
       </c>
@@ -1668,16 +1665,16 @@
         <v>45429</v>
       </c>
       <c r="E24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>5</v>
       </c>
@@ -1691,16 +1688,16 @@
         <v>45460</v>
       </c>
       <c r="E25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G25" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>6</v>
       </c>
@@ -1714,16 +1711,16 @@
         <v>45371</v>
       </c>
       <c r="E26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>6</v>
       </c>
@@ -1737,16 +1734,16 @@
         <v>45506</v>
       </c>
       <c r="E27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G27" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>6</v>
       </c>
@@ -1760,16 +1757,16 @@
         <v>45477</v>
       </c>
       <c r="E28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G28" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>6</v>
       </c>
@@ -1783,16 +1780,16 @@
         <v>45463</v>
       </c>
       <c r="E29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>6</v>
       </c>
@@ -1806,16 +1803,16 @@
         <v>45494</v>
       </c>
       <c r="E30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G30" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>7</v>
       </c>
@@ -1829,16 +1826,16 @@
         <v>45505</v>
       </c>
       <c r="E31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F31" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" t="s">
         <v>55</v>
       </c>
-      <c r="G31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>7</v>
       </c>
@@ -1852,16 +1849,16 @@
         <v>45297</v>
       </c>
       <c r="E32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>7</v>
       </c>
@@ -1875,16 +1872,16 @@
         <v>45328</v>
       </c>
       <c r="E33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G33" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>7</v>
       </c>
@@ -1898,16 +1895,16 @@
         <v>45571</v>
       </c>
       <c r="E34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G34" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>7</v>
       </c>
@@ -1921,16 +1918,16 @@
         <v>45446</v>
       </c>
       <c r="E35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>8</v>
       </c>
@@ -1944,16 +1941,16 @@
         <v>45534</v>
       </c>
       <c r="E36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F36" t="s">
+        <v>54</v>
+      </c>
+      <c r="G36" t="s">
         <v>55</v>
       </c>
-      <c r="G36" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>8</v>
       </c>
@@ -1967,16 +1964,16 @@
         <v>45292</v>
       </c>
       <c r="E37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G37" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>8</v>
       </c>
@@ -1990,16 +1987,16 @@
         <v>45529</v>
       </c>
       <c r="E38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G38" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>8</v>
       </c>
@@ -2013,16 +2010,16 @@
         <v>45483</v>
       </c>
       <c r="E39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F39" t="s">
+        <v>54</v>
+      </c>
+      <c r="G39" t="s">
         <v>55</v>
       </c>
-      <c r="G39" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>8</v>
       </c>
@@ -2036,16 +2033,16 @@
         <v>45421</v>
       </c>
       <c r="E40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G40" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>9</v>
       </c>
@@ -2059,16 +2056,16 @@
         <v>45316</v>
       </c>
       <c r="E41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G41" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>9</v>
       </c>
@@ -2082,16 +2079,16 @@
         <v>45366</v>
       </c>
       <c r="E42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G42" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>9</v>
       </c>
@@ -2105,16 +2102,16 @@
         <v>45512</v>
       </c>
       <c r="E43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G43" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>9</v>
       </c>
@@ -2128,16 +2125,16 @@
         <v>45378</v>
       </c>
       <c r="E44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G44" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>9</v>
       </c>
@@ -2151,16 +2148,16 @@
         <v>45384</v>
       </c>
       <c r="E45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G45" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>10</v>
       </c>
@@ -2174,16 +2171,16 @@
         <v>45502</v>
       </c>
       <c r="E46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G46" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>10</v>
       </c>
@@ -2197,16 +2194,16 @@
         <v>45465</v>
       </c>
       <c r="E47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F47" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G47" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>10</v>
       </c>
@@ -2220,16 +2217,16 @@
         <v>45327</v>
       </c>
       <c r="E48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G48" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>10</v>
       </c>
@@ -2243,16 +2240,16 @@
         <v>45323</v>
       </c>
       <c r="E49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G49" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>10</v>
       </c>
@@ -2266,13 +2263,13 @@
         <v>45416</v>
       </c>
       <c r="E50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F50" t="s">
+        <v>54</v>
+      </c>
+      <c r="G50" t="s">
         <v>55</v>
-      </c>
-      <c r="G50" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2288,12 +2285,12 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2313,7 +2310,7 @@
         <v>45610</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2333,7 +2330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2353,7 +2350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2373,7 +2370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2393,7 +2390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2413,7 +2410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2433,7 +2430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2453,7 +2450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2473,7 +2470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2493,7 +2490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2522,359 +2519,359 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B878E68-2103-EB43-B0E1-C1EADBE71D5E}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="42.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
         <v>80</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>81</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>82</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>83</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>84</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>85</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>86</v>
       </c>
-      <c r="H1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:8" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>45444</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" t="s">
         <v>88</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>89</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>90</v>
       </c>
-      <c r="F2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>45445</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" t="s">
         <v>92</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" t="s">
         <v>93</v>
       </c>
-      <c r="E3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:8" ht="216" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>45446</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" t="s">
         <v>95</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" t="s">
         <v>96</v>
       </c>
-      <c r="E4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:8" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>45447</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" t="s">
         <v>98</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" t="s">
         <v>99</v>
       </c>
-      <c r="E5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:8" ht="216" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>45448</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" t="s">
         <v>101</v>
       </c>
-      <c r="D6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:8" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>45449</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" t="s">
         <v>103</v>
       </c>
-      <c r="D7" t="s">
-        <v>93</v>
-      </c>
-      <c r="E7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:8" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>45450</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" t="s">
         <v>105</v>
       </c>
-      <c r="D8" t="s">
-        <v>96</v>
-      </c>
-      <c r="E8" t="s">
-        <v>90</v>
-      </c>
-      <c r="F8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>45451</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" t="s">
         <v>107</v>
       </c>
-      <c r="D9" t="s">
-        <v>99</v>
-      </c>
-      <c r="E9" t="s">
-        <v>90</v>
-      </c>
-      <c r="F9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:8" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>45452</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" t="s">
         <v>89</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>90</v>
       </c>
-      <c r="F10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:8" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>45453</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" t="s">
         <v>93</v>
       </c>
-      <c r="E11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:8" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>45454</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" t="s">
         <v>96</v>
       </c>
-      <c r="E12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:8" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>45455</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" t="s">
         <v>99</v>
       </c>
-      <c r="E13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:8" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>45456</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14" t="s">
         <v>89</v>
       </c>
-      <c r="E14" t="s">
-        <v>90</v>
-      </c>
       <c r="F14" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>45457</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>45458</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>45459</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>